<commit_message>
fix(salary): update salary excel
</commit_message>
<xml_diff>
--- a/src/main/resources/template/excel/salary.xlsx
+++ b/src/main/resources/template/excel/salary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\eclipse-workspace\erp\src\main\resources\template\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A79F667-55D6-48AB-833A-56B6A03F2875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5C5C94-C15B-41E9-9758-9DF749564991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10395" yWindow="3105" windowWidth="18405" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -142,10 +142,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>${G15 - G26}</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>$[SUM(G10:G14)]</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -207,6 +203,10 @@
   </si>
   <si>
     <t>${user.username}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>$[SUM(G15:G26)]</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -726,8 +726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G208"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D3"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -739,7 +739,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -760,12 +760,12 @@
     <row r="4" spans="1:7" ht="18" customHeight="1"/>
     <row r="5" spans="1:7" ht="21" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="24.75" customHeight="1">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="8.25" customHeight="1"/>
@@ -790,7 +790,7 @@
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="4" customFormat="1" ht="19.5">
@@ -802,19 +802,19 @@
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="4" customFormat="1" ht="19.5">
       <c r="B12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="4" customFormat="1" ht="19.5">
@@ -832,7 +832,7 @@
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="11" customFormat="1" ht="19.5">
@@ -841,7 +841,7 @@
       </c>
       <c r="F16" s="12"/>
       <c r="G16" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="4" customFormat="1" ht="19.5">
@@ -873,7 +873,7 @@
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="4" customFormat="1" ht="19.5">
@@ -885,7 +885,7 @@
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="4" customFormat="1" ht="19.5">
@@ -928,7 +928,7 @@
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="6" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="4" customFormat="1" ht="19.5">
@@ -973,26 +973,26 @@
     </row>
     <row r="35" spans="1:7" s="4" customFormat="1" ht="19.5">
       <c r="A35" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
     </row>
     <row r="36" spans="1:7" s="4" customFormat="1" ht="19.5">
       <c r="A36" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="E36" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="F36" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="G36" s="6"/>
     </row>

</xml_diff>

<commit_message>
fix(salary): update salary file output config
</commit_message>
<xml_diff>
--- a/src/main/resources/template/excel/salary.xlsx
+++ b/src/main/resources/template/excel/salary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\eclipse-workspace\erp\src\main\resources\template\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5C5C94-C15B-41E9-9758-9DF749564991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6D4DCA-9196-4EEA-8494-0D2C52229A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10395" yWindow="3105" windowWidth="18405" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,40 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>PC-603</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{8272FA9F-8BC8-4A5B-BBEA-770954B2FBFD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>PC-603:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:area(lastCell="I38")</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -218,7 +252,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="12"/>
       <name val="新細明體"/>
@@ -298,6 +332,19 @@
       <name val="新細明體"/>
       <family val="1"/>
       <charset val="136"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -723,11 +770,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1732,5 +1779,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix(file): update salary template file
</commit_message>
<xml_diff>
--- a/src/main/resources/template/excel/salary.xlsx
+++ b/src/main/resources/template/excel/salary.xlsx
@@ -1,32 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\eclipse-workspace\erp\src\main\resources\template\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\IdeaProjects\erp\src\main\resources\template\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6D4DCA-9196-4EEA-8494-0D2C52229A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D1A0A9-5D69-4767-A785-5866B4695001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -65,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Pay</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -168,18 +157,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>$[SUM(G26:G28)]</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>$[SUM(G21:G22)]</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>$[SUM(G10:G14)]</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Bonus</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -240,7 +217,11 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>$[SUM(G15:G26)]</t>
+    <t>${data.reduceTotal}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>${data.grandTotal}</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -252,7 +233,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <name val="新細明體"/>
@@ -316,12 +297,6 @@
     <font>
       <sz val="14"/>
       <color rgb="FFFF0000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FFFF0000"/>
       <name val="新細明體"/>
       <family val="1"/>
       <charset val="136"/>
@@ -377,7 +352,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -393,10 +368,9 @@
     <xf numFmtId="176" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -771,64 +745,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G208"/>
+  <dimension ref="A1:G203"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.2"/>
   <cols>
-    <col min="5" max="5" width="12.375" customWidth="1"/>
-    <col min="6" max="6" width="11.125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="12.5" style="5" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
+      <c r="A1" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
     </row>
     <row r="4" spans="1:7" ht="18" customHeight="1"/>
     <row r="5" spans="1:7" ht="21" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="24.75" customHeight="1">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="8.25" customHeight="1"/>
-    <row r="8" spans="1:7" s="4" customFormat="1" ht="19.5">
+    <row r="8" spans="1:7" s="4" customFormat="1" ht="19.8">
       <c r="A8" s="2"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" ht="19.5">
+    <row r="9" spans="1:7" s="4" customFormat="1" ht="19.8">
       <c r="A9" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:7" s="4" customFormat="1" ht="19.5">
+    <row r="10" spans="1:7" s="4" customFormat="1" ht="19.8">
       <c r="B10" s="2" t="s">
         <v>1</v>
       </c>
@@ -837,10 +811,10 @@
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="4" customFormat="1" ht="19.5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="4" customFormat="1" ht="19.8">
       <c r="B11" s="2" t="s">
         <v>3</v>
       </c>
@@ -849,867 +823,883 @@
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="4" customFormat="1" ht="19.5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="4" customFormat="1" ht="19.8">
       <c r="B12" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="4" customFormat="1" ht="19.5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="4" customFormat="1" ht="19.8">
       <c r="B13" s="13"/>
       <c r="F13" s="8"/>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" ht="19.5">
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="1:7" s="4" customFormat="1" ht="19.8">
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
     </row>
-    <row r="15" spans="1:7" s="4" customFormat="1" ht="19.5">
-      <c r="D15" s="2" t="s">
+    <row r="15" spans="1:7" s="4" customFormat="1" ht="19.8">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" s="11" customFormat="1" ht="19.5">
-      <c r="B16" s="11" t="s">
+      <c r="E15" s="10"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="11" customFormat="1" ht="19.8">
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="1:7" s="4" customFormat="1" ht="19.8">
+      <c r="A17" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="12"/>
-      <c r="G16" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" s="4" customFormat="1" ht="19.5">
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
     </row>
-    <row r="18" spans="1:7" s="4" customFormat="1" ht="19.5">
+    <row r="18" spans="1:7" s="4" customFormat="1" ht="19.8">
+      <c r="A18" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
     </row>
-    <row r="19" spans="1:7" s="4" customFormat="1" ht="19.5">
-      <c r="A19" s="3" t="s">
-        <v>5</v>
-      </c>
+    <row r="19" spans="1:7" s="4" customFormat="1" ht="19.8">
+      <c r="A19" s="3"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
     </row>
-    <row r="20" spans="1:7" s="4" customFormat="1" ht="19.5">
-      <c r="A20" s="3"/>
+    <row r="20" spans="1:7" s="4" customFormat="1" ht="19.8">
+      <c r="B20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-    </row>
-    <row r="21" spans="1:7" s="4" customFormat="1" ht="19.5">
+      <c r="G20" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="4" customFormat="1" ht="19.8">
       <c r="B21" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" s="4" customFormat="1" ht="19.5">
-      <c r="B22" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" s="4" customFormat="1" ht="19.5">
-      <c r="B23" s="13"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="4" customFormat="1" ht="19.8">
+      <c r="B22" s="13"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+    </row>
+    <row r="23" spans="1:7" s="4" customFormat="1" ht="19.8">
       <c r="F23" s="6"/>
-      <c r="G23" s="8"/>
-    </row>
-    <row r="24" spans="1:7" s="4" customFormat="1" ht="19.5">
-      <c r="B24" s="13"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="7"/>
-    </row>
-    <row r="25" spans="1:7" s="4" customFormat="1" ht="19.5">
+      <c r="G23" s="6"/>
+    </row>
+    <row r="24" spans="1:7" s="4" customFormat="1" ht="19.8">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="9"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="4" customFormat="1" ht="19.8">
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
     </row>
-    <row r="26" spans="1:7" s="4" customFormat="1" ht="19.5">
-      <c r="A26" s="9"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" s="4" customFormat="1" ht="19.5">
+    <row r="26" spans="1:7" s="4" customFormat="1" ht="19.8">
+      <c r="D26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="6"/>
+    </row>
+    <row r="27" spans="1:7" s="4" customFormat="1" ht="19.8">
+      <c r="D27" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-    </row>
-    <row r="28" spans="1:7" s="4" customFormat="1" ht="19.5">
-      <c r="D28" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" s="4" customFormat="1" ht="19.5">
+      <c r="G27" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="4" customFormat="1" ht="19.8">
+      <c r="A28" s="14"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+    </row>
+    <row r="29" spans="1:7" s="4" customFormat="1" ht="19.8">
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
     </row>
-    <row r="30" spans="1:7" s="4" customFormat="1" ht="19.5">
-      <c r="A30" s="15"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="17"/>
+    <row r="30" spans="1:7" s="4" customFormat="1" ht="19.8">
+      <c r="A30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" s="6"/>
       <c r="G30" s="6"/>
     </row>
-    <row r="31" spans="1:7" s="4" customFormat="1" ht="19.5">
-      <c r="A31" s="14"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="17"/>
+    <row r="31" spans="1:7" s="4" customFormat="1" ht="19.8">
+      <c r="A31" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="G31" s="6"/>
     </row>
-    <row r="32" spans="1:7" s="4" customFormat="1" ht="19.5">
-      <c r="A32" s="2"/>
+    <row r="32" spans="1:7" s="4" customFormat="1" ht="19.8">
+      <c r="A32" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="F32" s="6"/>
-      <c r="G32" s="7"/>
-    </row>
-    <row r="33" spans="1:7" s="4" customFormat="1" ht="19.5">
-      <c r="A33" s="13"/>
-      <c r="D33" s="4" t="s">
-        <v>15</v>
+      <c r="G32" s="6"/>
+    </row>
+    <row r="33" spans="1:7" s="4" customFormat="1" ht="19.8">
+      <c r="A33" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="F33" s="6"/>
-      <c r="G33" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" s="4" customFormat="1" ht="19.5">
+      <c r="G33" s="6"/>
+    </row>
+    <row r="34" spans="1:7" s="4" customFormat="1" ht="19.8">
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
     </row>
-    <row r="35" spans="1:7" s="4" customFormat="1" ht="19.5">
-      <c r="A35" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>28</v>
-      </c>
+    <row r="35" spans="1:7" s="4" customFormat="1" ht="19.8">
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
     </row>
-    <row r="36" spans="1:7" s="4" customFormat="1" ht="19.5">
-      <c r="A36" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>33</v>
-      </c>
+    <row r="36" spans="1:7" s="4" customFormat="1" ht="19.8">
+      <c r="F36" s="6"/>
       <c r="G36" s="6"/>
     </row>
-    <row r="37" spans="1:7" s="4" customFormat="1" ht="19.5">
-      <c r="A37" s="4" t="s">
-        <v>13</v>
-      </c>
+    <row r="37" spans="1:7" s="4" customFormat="1" ht="19.8">
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
     </row>
-    <row r="38" spans="1:7" s="4" customFormat="1" ht="19.5">
-      <c r="A38" s="4" t="s">
-        <v>16</v>
-      </c>
+    <row r="38" spans="1:7" s="4" customFormat="1" ht="19.8">
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
     </row>
-    <row r="39" spans="1:7" s="4" customFormat="1" ht="19.5">
+    <row r="39" spans="1:7" s="4" customFormat="1" ht="19.8">
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
     </row>
-    <row r="40" spans="1:7" s="4" customFormat="1" ht="19.5">
+    <row r="40" spans="1:7" s="4" customFormat="1" ht="19.8">
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
     </row>
-    <row r="41" spans="1:7" s="4" customFormat="1" ht="19.5">
+    <row r="41" spans="1:7" s="4" customFormat="1" ht="19.8">
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
     </row>
-    <row r="42" spans="1:7" s="4" customFormat="1" ht="19.5">
+    <row r="42" spans="1:7" s="4" customFormat="1" ht="19.8">
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
     </row>
-    <row r="43" spans="1:7" s="4" customFormat="1" ht="19.5">
+    <row r="43" spans="1:7" s="4" customFormat="1" ht="19.8">
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
     </row>
-    <row r="44" spans="1:7" s="4" customFormat="1" ht="19.5">
+    <row r="44" spans="1:7" s="4" customFormat="1" ht="19.8">
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
     </row>
-    <row r="45" spans="1:7" s="4" customFormat="1" ht="19.5">
+    <row r="45" spans="1:7" s="4" customFormat="1" ht="19.8">
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
     </row>
-    <row r="46" spans="1:7" s="4" customFormat="1" ht="19.5">
+    <row r="46" spans="1:7" s="4" customFormat="1" ht="19.8">
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
     </row>
-    <row r="47" spans="1:7" s="4" customFormat="1" ht="19.5">
+    <row r="47" spans="1:7" s="4" customFormat="1" ht="19.8">
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
     </row>
-    <row r="48" spans="1:7" s="4" customFormat="1" ht="19.5">
+    <row r="48" spans="1:7" s="4" customFormat="1" ht="19.8">
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
     </row>
-    <row r="49" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="49" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
     </row>
-    <row r="50" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="50" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
     </row>
-    <row r="51" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="51" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
     </row>
-    <row r="52" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="52" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
     </row>
-    <row r="53" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="53" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
     </row>
-    <row r="54" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="54" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F54" s="6"/>
       <c r="G54" s="6"/>
     </row>
-    <row r="55" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="55" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F55" s="6"/>
       <c r="G55" s="6"/>
     </row>
-    <row r="56" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="56" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
     </row>
-    <row r="57" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="57" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F57" s="6"/>
       <c r="G57" s="6"/>
     </row>
-    <row r="58" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="58" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F58" s="6"/>
       <c r="G58" s="6"/>
     </row>
-    <row r="59" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="59" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F59" s="6"/>
       <c r="G59" s="6"/>
     </row>
-    <row r="60" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="60" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F60" s="6"/>
       <c r="G60" s="6"/>
     </row>
-    <row r="61" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="61" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F61" s="6"/>
       <c r="G61" s="6"/>
     </row>
-    <row r="62" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="62" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F62" s="6"/>
       <c r="G62" s="6"/>
     </row>
-    <row r="63" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="63" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F63" s="6"/>
       <c r="G63" s="6"/>
     </row>
-    <row r="64" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="64" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F64" s="6"/>
       <c r="G64" s="6"/>
     </row>
-    <row r="65" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="65" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F65" s="6"/>
       <c r="G65" s="6"/>
     </row>
-    <row r="66" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="66" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F66" s="6"/>
       <c r="G66" s="6"/>
     </row>
-    <row r="67" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="67" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F67" s="6"/>
       <c r="G67" s="6"/>
     </row>
-    <row r="68" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="68" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F68" s="6"/>
       <c r="G68" s="6"/>
     </row>
-    <row r="69" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="69" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F69" s="6"/>
       <c r="G69" s="6"/>
     </row>
-    <row r="70" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="70" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F70" s="6"/>
       <c r="G70" s="6"/>
     </row>
-    <row r="71" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="71" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F71" s="6"/>
       <c r="G71" s="6"/>
     </row>
-    <row r="72" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="72" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F72" s="6"/>
       <c r="G72" s="6"/>
     </row>
-    <row r="73" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="73" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F73" s="6"/>
       <c r="G73" s="6"/>
     </row>
-    <row r="74" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="74" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F74" s="6"/>
       <c r="G74" s="6"/>
     </row>
-    <row r="75" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="75" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F75" s="6"/>
       <c r="G75" s="6"/>
     </row>
-    <row r="76" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="76" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F76" s="6"/>
       <c r="G76" s="6"/>
     </row>
-    <row r="77" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="77" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F77" s="6"/>
       <c r="G77" s="6"/>
     </row>
-    <row r="78" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="78" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F78" s="6"/>
       <c r="G78" s="6"/>
     </row>
-    <row r="79" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="79" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F79" s="6"/>
       <c r="G79" s="6"/>
     </row>
-    <row r="80" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="80" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F80" s="6"/>
       <c r="G80" s="6"/>
     </row>
-    <row r="81" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="81" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F81" s="6"/>
       <c r="G81" s="6"/>
     </row>
-    <row r="82" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="82" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F82" s="6"/>
       <c r="G82" s="6"/>
     </row>
-    <row r="83" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="83" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F83" s="6"/>
       <c r="G83" s="6"/>
     </row>
-    <row r="84" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="84" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F84" s="6"/>
       <c r="G84" s="6"/>
     </row>
-    <row r="85" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="85" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F85" s="6"/>
       <c r="G85" s="6"/>
     </row>
-    <row r="86" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="86" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F86" s="6"/>
       <c r="G86" s="6"/>
     </row>
-    <row r="87" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="87" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F87" s="6"/>
       <c r="G87" s="6"/>
     </row>
-    <row r="88" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="88" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F88" s="6"/>
       <c r="G88" s="6"/>
     </row>
-    <row r="89" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="89" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F89" s="6"/>
       <c r="G89" s="6"/>
     </row>
-    <row r="90" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="90" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F90" s="6"/>
       <c r="G90" s="6"/>
     </row>
-    <row r="91" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="91" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F91" s="6"/>
       <c r="G91" s="6"/>
     </row>
-    <row r="92" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="92" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F92" s="6"/>
       <c r="G92" s="6"/>
     </row>
-    <row r="93" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="93" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F93" s="6"/>
       <c r="G93" s="6"/>
     </row>
-    <row r="94" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="94" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F94" s="6"/>
       <c r="G94" s="6"/>
     </row>
-    <row r="95" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="95" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F95" s="6"/>
       <c r="G95" s="6"/>
     </row>
-    <row r="96" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="96" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F96" s="6"/>
       <c r="G96" s="6"/>
     </row>
-    <row r="97" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="97" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F97" s="6"/>
       <c r="G97" s="6"/>
     </row>
-    <row r="98" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="98" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F98" s="6"/>
       <c r="G98" s="6"/>
     </row>
-    <row r="99" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="99" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F99" s="6"/>
       <c r="G99" s="6"/>
     </row>
-    <row r="100" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="100" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F100" s="6"/>
       <c r="G100" s="6"/>
     </row>
-    <row r="101" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="101" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F101" s="6"/>
       <c r="G101" s="6"/>
     </row>
-    <row r="102" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="102" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F102" s="6"/>
       <c r="G102" s="6"/>
     </row>
-    <row r="103" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="103" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F103" s="6"/>
       <c r="G103" s="6"/>
     </row>
-    <row r="104" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="104" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F104" s="6"/>
       <c r="G104" s="6"/>
     </row>
-    <row r="105" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="105" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F105" s="6"/>
       <c r="G105" s="6"/>
     </row>
-    <row r="106" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="106" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F106" s="6"/>
       <c r="G106" s="6"/>
     </row>
-    <row r="107" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="107" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F107" s="6"/>
       <c r="G107" s="6"/>
     </row>
-    <row r="108" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="108" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F108" s="6"/>
       <c r="G108" s="6"/>
     </row>
-    <row r="109" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="109" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F109" s="6"/>
       <c r="G109" s="6"/>
     </row>
-    <row r="110" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="110" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F110" s="6"/>
       <c r="G110" s="6"/>
     </row>
-    <row r="111" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="111" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F111" s="6"/>
       <c r="G111" s="6"/>
     </row>
-    <row r="112" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="112" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F112" s="6"/>
       <c r="G112" s="6"/>
     </row>
-    <row r="113" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="113" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F113" s="6"/>
       <c r="G113" s="6"/>
     </row>
-    <row r="114" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="114" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F114" s="6"/>
       <c r="G114" s="6"/>
     </row>
-    <row r="115" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="115" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F115" s="6"/>
       <c r="G115" s="6"/>
     </row>
-    <row r="116" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="116" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F116" s="6"/>
       <c r="G116" s="6"/>
     </row>
-    <row r="117" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="117" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F117" s="6"/>
       <c r="G117" s="6"/>
     </row>
-    <row r="118" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="118" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F118" s="6"/>
       <c r="G118" s="6"/>
     </row>
-    <row r="119" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="119" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F119" s="6"/>
       <c r="G119" s="6"/>
     </row>
-    <row r="120" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="120" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F120" s="6"/>
       <c r="G120" s="6"/>
     </row>
-    <row r="121" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="121" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F121" s="6"/>
       <c r="G121" s="6"/>
     </row>
-    <row r="122" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="122" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F122" s="6"/>
       <c r="G122" s="6"/>
     </row>
-    <row r="123" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="123" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F123" s="6"/>
       <c r="G123" s="6"/>
     </row>
-    <row r="124" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="124" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F124" s="6"/>
       <c r="G124" s="6"/>
     </row>
-    <row r="125" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="125" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F125" s="6"/>
       <c r="G125" s="6"/>
     </row>
-    <row r="126" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="126" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F126" s="6"/>
       <c r="G126" s="6"/>
     </row>
-    <row r="127" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="127" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F127" s="6"/>
       <c r="G127" s="6"/>
     </row>
-    <row r="128" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="128" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F128" s="6"/>
       <c r="G128" s="6"/>
     </row>
-    <row r="129" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="129" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F129" s="6"/>
       <c r="G129" s="6"/>
     </row>
-    <row r="130" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="130" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F130" s="6"/>
       <c r="G130" s="6"/>
     </row>
-    <row r="131" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="131" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F131" s="6"/>
       <c r="G131" s="6"/>
     </row>
-    <row r="132" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="132" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F132" s="6"/>
       <c r="G132" s="6"/>
     </row>
-    <row r="133" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="133" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F133" s="6"/>
       <c r="G133" s="6"/>
     </row>
-    <row r="134" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="134" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F134" s="6"/>
       <c r="G134" s="6"/>
     </row>
-    <row r="135" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="135" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F135" s="6"/>
       <c r="G135" s="6"/>
     </row>
-    <row r="136" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="136" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F136" s="6"/>
       <c r="G136" s="6"/>
     </row>
-    <row r="137" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="137" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F137" s="6"/>
       <c r="G137" s="6"/>
     </row>
-    <row r="138" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="138" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F138" s="6"/>
       <c r="G138" s="6"/>
     </row>
-    <row r="139" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="139" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F139" s="6"/>
       <c r="G139" s="6"/>
     </row>
-    <row r="140" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="140" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F140" s="6"/>
       <c r="G140" s="6"/>
     </row>
-    <row r="141" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="141" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F141" s="6"/>
       <c r="G141" s="6"/>
     </row>
-    <row r="142" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="142" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F142" s="6"/>
       <c r="G142" s="6"/>
     </row>
-    <row r="143" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="143" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F143" s="6"/>
       <c r="G143" s="6"/>
     </row>
-    <row r="144" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="144" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F144" s="6"/>
       <c r="G144" s="6"/>
     </row>
-    <row r="145" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="145" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F145" s="6"/>
       <c r="G145" s="6"/>
     </row>
-    <row r="146" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="146" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F146" s="6"/>
       <c r="G146" s="6"/>
     </row>
-    <row r="147" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="147" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F147" s="6"/>
       <c r="G147" s="6"/>
     </row>
-    <row r="148" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="148" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F148" s="6"/>
       <c r="G148" s="6"/>
     </row>
-    <row r="149" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="149" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F149" s="6"/>
       <c r="G149" s="6"/>
     </row>
-    <row r="150" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="150" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F150" s="6"/>
       <c r="G150" s="6"/>
     </row>
-    <row r="151" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="151" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F151" s="6"/>
       <c r="G151" s="6"/>
     </row>
-    <row r="152" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="152" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F152" s="6"/>
       <c r="G152" s="6"/>
     </row>
-    <row r="153" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="153" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F153" s="6"/>
       <c r="G153" s="6"/>
     </row>
-    <row r="154" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="154" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F154" s="6"/>
       <c r="G154" s="6"/>
     </row>
-    <row r="155" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="155" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F155" s="6"/>
       <c r="G155" s="6"/>
     </row>
-    <row r="156" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="156" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F156" s="6"/>
       <c r="G156" s="6"/>
     </row>
-    <row r="157" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="157" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F157" s="6"/>
       <c r="G157" s="6"/>
     </row>
-    <row r="158" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="158" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F158" s="6"/>
       <c r="G158" s="6"/>
     </row>
-    <row r="159" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="159" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F159" s="6"/>
       <c r="G159" s="6"/>
     </row>
-    <row r="160" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="160" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F160" s="6"/>
       <c r="G160" s="6"/>
     </row>
-    <row r="161" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="161" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F161" s="6"/>
       <c r="G161" s="6"/>
     </row>
-    <row r="162" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="162" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F162" s="6"/>
       <c r="G162" s="6"/>
     </row>
-    <row r="163" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="163" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F163" s="6"/>
       <c r="G163" s="6"/>
     </row>
-    <row r="164" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="164" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F164" s="6"/>
       <c r="G164" s="6"/>
     </row>
-    <row r="165" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="165" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F165" s="6"/>
       <c r="G165" s="6"/>
     </row>
-    <row r="166" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="166" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F166" s="6"/>
       <c r="G166" s="6"/>
     </row>
-    <row r="167" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="167" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F167" s="6"/>
       <c r="G167" s="6"/>
     </row>
-    <row r="168" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="168" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F168" s="6"/>
       <c r="G168" s="6"/>
     </row>
-    <row r="169" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="169" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F169" s="6"/>
       <c r="G169" s="6"/>
     </row>
-    <row r="170" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="170" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F170" s="6"/>
       <c r="G170" s="6"/>
     </row>
-    <row r="171" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="171" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F171" s="6"/>
       <c r="G171" s="6"/>
     </row>
-    <row r="172" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="172" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F172" s="6"/>
       <c r="G172" s="6"/>
     </row>
-    <row r="173" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="173" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F173" s="6"/>
       <c r="G173" s="6"/>
     </row>
-    <row r="174" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="174" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F174" s="6"/>
       <c r="G174" s="6"/>
     </row>
-    <row r="175" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="175" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F175" s="6"/>
       <c r="G175" s="6"/>
     </row>
-    <row r="176" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="176" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F176" s="6"/>
       <c r="G176" s="6"/>
     </row>
-    <row r="177" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="177" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F177" s="6"/>
       <c r="G177" s="6"/>
     </row>
-    <row r="178" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="178" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F178" s="6"/>
       <c r="G178" s="6"/>
     </row>
-    <row r="179" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="179" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F179" s="6"/>
       <c r="G179" s="6"/>
     </row>
-    <row r="180" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="180" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F180" s="6"/>
       <c r="G180" s="6"/>
     </row>
-    <row r="181" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="181" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F181" s="6"/>
       <c r="G181" s="6"/>
     </row>
-    <row r="182" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="182" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F182" s="6"/>
       <c r="G182" s="6"/>
     </row>
-    <row r="183" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="183" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F183" s="6"/>
       <c r="G183" s="6"/>
     </row>
-    <row r="184" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="184" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F184" s="6"/>
       <c r="G184" s="6"/>
     </row>
-    <row r="185" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="185" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F185" s="6"/>
       <c r="G185" s="6"/>
     </row>
-    <row r="186" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="186" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F186" s="6"/>
       <c r="G186" s="6"/>
     </row>
-    <row r="187" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="187" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F187" s="6"/>
       <c r="G187" s="6"/>
     </row>
-    <row r="188" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="188" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F188" s="6"/>
       <c r="G188" s="6"/>
     </row>
-    <row r="189" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="189" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F189" s="6"/>
       <c r="G189" s="6"/>
     </row>
-    <row r="190" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="190" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F190" s="6"/>
       <c r="G190" s="6"/>
     </row>
-    <row r="191" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="191" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F191" s="6"/>
       <c r="G191" s="6"/>
     </row>
-    <row r="192" spans="6:7" s="4" customFormat="1" ht="19.5">
+    <row r="192" spans="6:7" s="4" customFormat="1" ht="19.8">
       <c r="F192" s="6"/>
       <c r="G192" s="6"/>
     </row>
-    <row r="193" spans="1:7" s="4" customFormat="1" ht="19.5">
+    <row r="193" spans="1:7" s="4" customFormat="1" ht="19.8">
       <c r="F193" s="6"/>
       <c r="G193" s="6"/>
     </row>
-    <row r="194" spans="1:7" s="4" customFormat="1" ht="19.5">
+    <row r="194" spans="1:7" s="4" customFormat="1" ht="19.8">
       <c r="F194" s="6"/>
       <c r="G194" s="6"/>
     </row>
-    <row r="195" spans="1:7" s="4" customFormat="1" ht="19.5">
+    <row r="195" spans="1:7" s="4" customFormat="1" ht="19.8">
       <c r="F195" s="6"/>
       <c r="G195" s="6"/>
     </row>
-    <row r="196" spans="1:7" s="4" customFormat="1" ht="19.5">
+    <row r="196" spans="1:7" s="4" customFormat="1" ht="19.8">
       <c r="F196" s="6"/>
       <c r="G196" s="6"/>
     </row>
-    <row r="197" spans="1:7" s="4" customFormat="1" ht="19.5">
+    <row r="197" spans="1:7" ht="19.8">
+      <c r="A197" s="4"/>
+      <c r="B197" s="4"/>
+      <c r="C197" s="4"/>
+      <c r="D197" s="4"/>
+      <c r="E197" s="4"/>
       <c r="F197" s="6"/>
       <c r="G197" s="6"/>
     </row>
-    <row r="198" spans="1:7" s="4" customFormat="1" ht="19.5">
+    <row r="198" spans="1:7" ht="19.8">
+      <c r="A198" s="4"/>
+      <c r="B198" s="4"/>
+      <c r="C198" s="4"/>
+      <c r="D198" s="4"/>
+      <c r="E198" s="4"/>
       <c r="F198" s="6"/>
       <c r="G198" s="6"/>
     </row>
-    <row r="199" spans="1:7" s="4" customFormat="1" ht="19.5">
+    <row r="199" spans="1:7" ht="19.8">
+      <c r="A199" s="4"/>
+      <c r="B199" s="4"/>
+      <c r="C199" s="4"/>
+      <c r="D199" s="4"/>
+      <c r="E199" s="4"/>
       <c r="F199" s="6"/>
       <c r="G199" s="6"/>
     </row>
-    <row r="200" spans="1:7" s="4" customFormat="1" ht="19.5">
+    <row r="200" spans="1:7" ht="19.8">
+      <c r="A200" s="4"/>
+      <c r="B200" s="4"/>
+      <c r="C200" s="4"/>
+      <c r="D200" s="4"/>
+      <c r="E200" s="4"/>
       <c r="F200" s="6"/>
       <c r="G200" s="6"/>
     </row>
-    <row r="201" spans="1:7" s="4" customFormat="1" ht="19.5">
+    <row r="201" spans="1:7" ht="19.8">
+      <c r="A201" s="4"/>
+      <c r="B201" s="4"/>
+      <c r="C201" s="4"/>
+      <c r="D201" s="4"/>
+      <c r="E201" s="4"/>
       <c r="F201" s="6"/>
       <c r="G201" s="6"/>
     </row>
-    <row r="202" spans="1:7" ht="19.5">
+    <row r="202" spans="1:7" ht="19.8">
       <c r="A202" s="4"/>
       <c r="B202" s="4"/>
       <c r="C202" s="4"/>
@@ -1718,58 +1708,13 @@
       <c r="F202" s="6"/>
       <c r="G202" s="6"/>
     </row>
-    <row r="203" spans="1:7" ht="19.5">
-      <c r="A203" s="4"/>
+    <row r="203" spans="1:7" ht="19.8">
       <c r="B203" s="4"/>
       <c r="C203" s="4"/>
       <c r="D203" s="4"/>
       <c r="E203" s="4"/>
       <c r="F203" s="6"/>
       <c r="G203" s="6"/>
-    </row>
-    <row r="204" spans="1:7" ht="19.5">
-      <c r="A204" s="4"/>
-      <c r="B204" s="4"/>
-      <c r="C204" s="4"/>
-      <c r="D204" s="4"/>
-      <c r="E204" s="4"/>
-      <c r="F204" s="6"/>
-      <c r="G204" s="6"/>
-    </row>
-    <row r="205" spans="1:7" ht="19.5">
-      <c r="A205" s="4"/>
-      <c r="B205" s="4"/>
-      <c r="C205" s="4"/>
-      <c r="D205" s="4"/>
-      <c r="E205" s="4"/>
-      <c r="F205" s="6"/>
-      <c r="G205" s="6"/>
-    </row>
-    <row r="206" spans="1:7" ht="19.5">
-      <c r="A206" s="4"/>
-      <c r="B206" s="4"/>
-      <c r="C206" s="4"/>
-      <c r="D206" s="4"/>
-      <c r="E206" s="4"/>
-      <c r="F206" s="6"/>
-      <c r="G206" s="6"/>
-    </row>
-    <row r="207" spans="1:7" ht="19.5">
-      <c r="A207" s="4"/>
-      <c r="B207" s="4"/>
-      <c r="C207" s="4"/>
-      <c r="D207" s="4"/>
-      <c r="E207" s="4"/>
-      <c r="F207" s="6"/>
-      <c r="G207" s="6"/>
-    </row>
-    <row r="208" spans="1:7" ht="19.5">
-      <c r="B208" s="4"/>
-      <c r="C208" s="4"/>
-      <c r="D208" s="4"/>
-      <c r="E208" s="4"/>
-      <c r="F208" s="6"/>
-      <c r="G208" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>